<commit_message>
Update as per execution and model definition
</commit_message>
<xml_diff>
--- a/data/layers_to_tensor_map.xlsx
+++ b/data/layers_to_tensor_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinay/workspace/upwork/tflite_models/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4872E5B4-6EB2-2E47-84C4-D77ADD0BCC1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDDCB07-1841-F844-B574-812A8CCF1266}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="layers" sheetId="3" r:id="rId1"/>
@@ -1392,7 +1392,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1528,6 +1528,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1989,7 +1996,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2045,15 +2052,6 @@
     <xf numFmtId="0" fontId="17" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2096,6 +2094,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2478,21 +2492,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCD4082-EE78-E549-A159-CF34924045AA}">
   <dimension ref="A1:F174"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F174" sqref="F3:F174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.33203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.33203125" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="90.33203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="90.33203125" style="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="35" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="32" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>240</v>
       </c>
@@ -2516,7 +2530,7 @@
       <c r="A2" s="18">
         <v>171</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>235</v>
       </c>
       <c r="C2" s="18" t="s">
@@ -2528,7 +2542,7 @@
       <c r="E2" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="19" t="s">
         <v>396</v>
       </c>
     </row>
@@ -2536,7 +2550,7 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -2548,7 +2562,7 @@
       <c r="E3" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="20" t="s">
         <v>280</v>
       </c>
     </row>
@@ -2556,7 +2570,7 @@
       <c r="A4" s="8">
         <v>0</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="20" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -2568,7 +2582,7 @@
       <c r="E4" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="20" t="s">
         <v>399</v>
       </c>
     </row>
@@ -2576,7 +2590,7 @@
       <c r="A5" s="8">
         <v>1</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -2588,7 +2602,7 @@
       <c r="E5" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="20" t="s">
         <v>279</v>
       </c>
     </row>
@@ -2596,7 +2610,7 @@
       <c r="A6" s="6">
         <v>13</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -2608,7 +2622,7 @@
       <c r="E6" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="21" t="s">
         <v>287</v>
       </c>
     </row>
@@ -2616,7 +2630,7 @@
       <c r="A7" s="6">
         <v>12</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="21" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -2628,7 +2642,7 @@
       <c r="E7" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="21" t="s">
         <v>403</v>
       </c>
     </row>
@@ -2636,7 +2650,7 @@
       <c r="A8" s="6">
         <v>11</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="21" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -2648,7 +2662,7 @@
       <c r="E8" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="21" t="s">
         <v>286</v>
       </c>
     </row>
@@ -2656,7 +2670,7 @@
       <c r="A9" s="6">
         <v>16</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -2668,7 +2682,7 @@
       <c r="E9" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="21" t="s">
         <v>289</v>
       </c>
     </row>
@@ -2676,7 +2690,7 @@
       <c r="A10" s="6">
         <v>14</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="21" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -2688,7 +2702,7 @@
       <c r="E10" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="21" t="s">
         <v>404</v>
       </c>
     </row>
@@ -2696,7 +2710,7 @@
       <c r="A11" s="6">
         <v>15</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -2708,19 +2722,19 @@
       <c r="E11" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="21" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
-        <v>19</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D12" s="12">
         <v>2</v>
@@ -2728,16 +2742,16 @@
       <c r="E12" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F12" s="25" t="s">
-        <v>291</v>
+      <c r="F12" s="22" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="12">
-        <v>18</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>34</v>
+        <v>20</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>38</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>35</v>
@@ -2748,19 +2762,19 @@
       <c r="E13" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F13" s="25" t="s">
-        <v>405</v>
+      <c r="F13" s="22" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="12">
-        <v>17</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>39</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D14" s="12">
         <v>2</v>
@@ -2768,19 +2782,19 @@
       <c r="E14" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F14" s="25" t="s">
-        <v>290</v>
+      <c r="F14" s="22" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="12">
-        <v>22</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>41</v>
+        <v>19</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>36</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D15" s="12">
         <v>2</v>
@@ -2788,16 +2802,16 @@
       <c r="E15" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F15" s="25" t="s">
-        <v>293</v>
+      <c r="F15" s="22" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="12">
-        <v>20</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>38</v>
+        <v>18</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>34</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>35</v>
@@ -2808,19 +2822,19 @@
       <c r="E16" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F16" s="25" t="s">
-        <v>406</v>
+      <c r="F16" s="22" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
-        <v>21</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>39</v>
+        <v>17</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D17" s="12">
         <v>2</v>
@@ -2828,15 +2842,15 @@
       <c r="E17" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F17" s="25" t="s">
-        <v>292</v>
+      <c r="F17" s="22" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
         <v>25</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="22" t="s">
         <v>47</v>
       </c>
       <c r="C18" s="12" t="s">
@@ -2848,7 +2862,7 @@
       <c r="E18" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F18" s="25" t="s">
+      <c r="F18" s="22" t="s">
         <v>295</v>
       </c>
     </row>
@@ -2856,7 +2870,7 @@
       <c r="A19" s="12">
         <v>23</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="22" t="s">
         <v>43</v>
       </c>
       <c r="C19" s="12" t="s">
@@ -2868,7 +2882,7 @@
       <c r="E19" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="22" t="s">
         <v>407</v>
       </c>
     </row>
@@ -2876,7 +2890,7 @@
       <c r="A20" s="12">
         <v>24</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="22" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="12" t="s">
@@ -2888,19 +2902,19 @@
       <c r="E20" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="22" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="12">
-        <v>96</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>144</v>
+        <v>99</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>148</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D21" s="12">
         <v>2</v>
@@ -2908,16 +2922,16 @@
       <c r="E21" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F21" s="25" t="s">
-        <v>344</v>
+      <c r="F21" s="22" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="12">
-        <v>95</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>142</v>
+        <v>97</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>146</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>143</v>
@@ -2928,16 +2942,16 @@
       <c r="E22" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F22" s="25" t="s">
-        <v>429</v>
+      <c r="F22" s="22" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
-        <v>94</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>140</v>
+        <v>98</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>147</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>141</v>
@@ -2948,19 +2962,19 @@
       <c r="E23" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F23" s="25" t="s">
-        <v>343</v>
+      <c r="F23" s="22" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="12">
-        <v>99</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>148</v>
+        <v>96</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>144</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D24" s="12">
         <v>2</v>
@@ -2968,16 +2982,16 @@
       <c r="E24" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F24" s="25" t="s">
-        <v>346</v>
+      <c r="F24" s="22" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="12">
-        <v>97</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>146</v>
+        <v>95</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>143</v>
@@ -2988,16 +3002,16 @@
       <c r="E25" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F25" s="25" t="s">
-        <v>430</v>
+      <c r="F25" s="22" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="12">
-        <v>98</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>147</v>
+        <v>94</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>140</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>141</v>
@@ -3008,15 +3022,15 @@
       <c r="E26" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F26" s="25" t="s">
-        <v>345</v>
+      <c r="F26" s="22" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="12">
         <v>102</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="22" t="s">
         <v>152</v>
       </c>
       <c r="C27" s="12" t="s">
@@ -3028,7 +3042,7 @@
       <c r="E27" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F27" s="25" t="s">
+      <c r="F27" s="22" t="s">
         <v>348</v>
       </c>
     </row>
@@ -3036,7 +3050,7 @@
       <c r="A28" s="12">
         <v>100</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="22" t="s">
         <v>150</v>
       </c>
       <c r="C28" s="12" t="s">
@@ -3048,7 +3062,7 @@
       <c r="E28" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F28" s="25" t="s">
+      <c r="F28" s="22" t="s">
         <v>431</v>
       </c>
     </row>
@@ -3056,7 +3070,7 @@
       <c r="A29" s="12">
         <v>101</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="22" t="s">
         <v>151</v>
       </c>
       <c r="C29" s="12" t="s">
@@ -3068,7 +3082,7 @@
       <c r="E29" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F29" s="25" t="s">
+      <c r="F29" s="22" t="s">
         <v>347</v>
       </c>
     </row>
@@ -3076,7 +3090,7 @@
       <c r="A30" s="12">
         <v>93</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="22" t="s">
         <v>139</v>
       </c>
       <c r="C30" s="12" t="s">
@@ -3088,19 +3102,19 @@
       <c r="E30" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F30" s="25" t="s">
+      <c r="F30" s="22" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="16">
-        <v>105</v>
-      </c>
-      <c r="B31" s="26" t="s">
-        <v>157</v>
+        <v>108</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>160</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D31" s="16">
         <v>3</v>
@@ -3108,16 +3122,16 @@
       <c r="E31" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F31" s="26" t="s">
-        <v>350</v>
+      <c r="F31" s="23" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="16">
-        <v>104</v>
-      </c>
-      <c r="B32" s="26" t="s">
-        <v>156</v>
+        <v>106</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>158</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>143</v>
@@ -3128,19 +3142,19 @@
       <c r="E32" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F32" s="26" t="s">
-        <v>432</v>
+      <c r="F32" s="23" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="16">
-        <v>103</v>
-      </c>
-      <c r="B33" s="26" t="s">
-        <v>154</v>
+        <v>107</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>159</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="D33" s="16">
         <v>3</v>
@@ -3148,19 +3162,19 @@
       <c r="E33" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F33" s="26" t="s">
-        <v>349</v>
+      <c r="F33" s="23" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="16">
-        <v>108</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>160</v>
+        <v>105</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>157</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D34" s="16">
         <v>3</v>
@@ -3168,16 +3182,16 @@
       <c r="E34" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F34" s="26" t="s">
-        <v>352</v>
+      <c r="F34" s="23" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="16">
-        <v>106</v>
-      </c>
-      <c r="B35" s="26" t="s">
-        <v>158</v>
+        <v>104</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>156</v>
       </c>
       <c r="C35" s="16" t="s">
         <v>143</v>
@@ -3188,19 +3202,19 @@
       <c r="E35" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F35" s="26" t="s">
-        <v>433</v>
+      <c r="F35" s="23" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="16">
-        <v>107</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>159</v>
+        <v>103</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>154</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="D36" s="16">
         <v>3</v>
@@ -3208,15 +3222,15 @@
       <c r="E36" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F36" s="26" t="s">
-        <v>351</v>
+      <c r="F36" s="23" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="16">
         <v>111</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="23" t="s">
         <v>164</v>
       </c>
       <c r="C37" s="16" t="s">
@@ -3228,7 +3242,7 @@
       <c r="E37" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F37" s="26" t="s">
+      <c r="F37" s="23" t="s">
         <v>354</v>
       </c>
     </row>
@@ -3236,7 +3250,7 @@
       <c r="A38" s="16">
         <v>109</v>
       </c>
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="23" t="s">
         <v>161</v>
       </c>
       <c r="C38" s="16" t="s">
@@ -3248,7 +3262,7 @@
       <c r="E38" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F38" s="26" t="s">
+      <c r="F38" s="23" t="s">
         <v>434</v>
       </c>
     </row>
@@ -3256,7 +3270,7 @@
       <c r="A39" s="16">
         <v>110</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="23" t="s">
         <v>162</v>
       </c>
       <c r="C39" s="16" t="s">
@@ -3268,19 +3282,19 @@
       <c r="E39" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F39" s="26" t="s">
+      <c r="F39" s="23" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="16">
-        <v>115</v>
-      </c>
-      <c r="B40" s="26" t="s">
-        <v>171</v>
+        <v>118</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>175</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D40" s="16">
         <v>3</v>
@@ -3288,16 +3302,16 @@
       <c r="E40" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F40" s="26" t="s">
-        <v>357</v>
+      <c r="F40" s="23" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="16">
-        <v>114</v>
-      </c>
-      <c r="B41" s="26" t="s">
-        <v>169</v>
+        <v>116</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>173</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>170</v>
@@ -3308,16 +3322,16 @@
       <c r="E41" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F41" s="26" t="s">
-        <v>435</v>
+      <c r="F41" s="23" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="16">
-        <v>113</v>
-      </c>
-      <c r="B42" s="26" t="s">
-        <v>167</v>
+        <v>117</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>174</v>
       </c>
       <c r="C42" s="16" t="s">
         <v>168</v>
@@ -3328,19 +3342,19 @@
       <c r="E42" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F42" s="26" t="s">
-        <v>356</v>
+      <c r="F42" s="23" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="16">
-        <v>118</v>
-      </c>
-      <c r="B43" s="26" t="s">
-        <v>175</v>
+        <v>115</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>171</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D43" s="16">
         <v>3</v>
@@ -3348,16 +3362,16 @@
       <c r="E43" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F43" s="26" t="s">
-        <v>359</v>
+      <c r="F43" s="23" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="16">
-        <v>116</v>
-      </c>
-      <c r="B44" s="26" t="s">
-        <v>173</v>
+        <v>114</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>169</v>
       </c>
       <c r="C44" s="16" t="s">
         <v>170</v>
@@ -3368,16 +3382,16 @@
       <c r="E44" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F44" s="26" t="s">
-        <v>436</v>
+      <c r="F44" s="23" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="16">
-        <v>117</v>
-      </c>
-      <c r="B45" s="26" t="s">
-        <v>174</v>
+        <v>113</v>
+      </c>
+      <c r="B45" s="23" t="s">
+        <v>167</v>
       </c>
       <c r="C45" s="16" t="s">
         <v>168</v>
@@ -3388,15 +3402,15 @@
       <c r="E45" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F45" s="26" t="s">
-        <v>358</v>
+      <c r="F45" s="23" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="16">
         <v>121</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="23" t="s">
         <v>179</v>
       </c>
       <c r="C46" s="16" t="s">
@@ -3408,7 +3422,7 @@
       <c r="E46" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F46" s="26" t="s">
+      <c r="F46" s="23" t="s">
         <v>361</v>
       </c>
     </row>
@@ -3416,7 +3430,7 @@
       <c r="A47" s="16">
         <v>119</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="23" t="s">
         <v>177</v>
       </c>
       <c r="C47" s="16" t="s">
@@ -3428,7 +3442,7 @@
       <c r="E47" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F47" s="26" t="s">
+      <c r="F47" s="23" t="s">
         <v>437</v>
       </c>
     </row>
@@ -3436,7 +3450,7 @@
       <c r="A48" s="16">
         <v>120</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="23" t="s">
         <v>178</v>
       </c>
       <c r="C48" s="16" t="s">
@@ -3448,7 +3462,7 @@
       <c r="E48" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F48" s="26" t="s">
+      <c r="F48" s="23" t="s">
         <v>360</v>
       </c>
     </row>
@@ -3456,7 +3470,7 @@
       <c r="A49" s="16">
         <v>112</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="23" t="s">
         <v>166</v>
       </c>
       <c r="C49" s="16" t="s">
@@ -3468,19 +3482,19 @@
       <c r="E49" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F49" s="26" t="s">
+      <c r="F49" s="23" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="16">
-        <v>125</v>
-      </c>
-      <c r="B50" s="26" t="s">
-        <v>184</v>
+        <v>128</v>
+      </c>
+      <c r="B50" s="23" t="s">
+        <v>187</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D50" s="16">
         <v>3</v>
@@ -3488,16 +3502,16 @@
       <c r="E50" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F50" s="26" t="s">
-        <v>364</v>
+      <c r="F50" s="23" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="16">
-        <v>124</v>
-      </c>
-      <c r="B51" s="26" t="s">
-        <v>183</v>
+        <v>126</v>
+      </c>
+      <c r="B51" s="23" t="s">
+        <v>185</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>170</v>
@@ -3508,16 +3522,16 @@
       <c r="E51" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F51" s="26" t="s">
-        <v>438</v>
+      <c r="F51" s="23" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="16">
-        <v>123</v>
-      </c>
-      <c r="B52" s="26" t="s">
-        <v>182</v>
+        <v>127</v>
+      </c>
+      <c r="B52" s="23" t="s">
+        <v>186</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>168</v>
@@ -3528,19 +3542,19 @@
       <c r="E52" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F52" s="26" t="s">
-        <v>363</v>
+      <c r="F52" s="23" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="16">
-        <v>128</v>
-      </c>
-      <c r="B53" s="26" t="s">
-        <v>187</v>
+        <v>125</v>
+      </c>
+      <c r="B53" s="23" t="s">
+        <v>184</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D53" s="16">
         <v>3</v>
@@ -3548,16 +3562,16 @@
       <c r="E53" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F53" s="26" t="s">
-        <v>366</v>
+      <c r="F53" s="23" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="16">
-        <v>126</v>
-      </c>
-      <c r="B54" s="26" t="s">
-        <v>185</v>
+        <v>124</v>
+      </c>
+      <c r="B54" s="23" t="s">
+        <v>183</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>170</v>
@@ -3568,16 +3582,16 @@
       <c r="E54" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F54" s="26" t="s">
-        <v>439</v>
+      <c r="F54" s="23" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="16">
-        <v>127</v>
-      </c>
-      <c r="B55" s="26" t="s">
-        <v>186</v>
+        <v>123</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>182</v>
       </c>
       <c r="C55" s="16" t="s">
         <v>168</v>
@@ -3588,15 +3602,15 @@
       <c r="E55" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F55" s="26" t="s">
-        <v>365</v>
+      <c r="F55" s="23" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="16">
         <v>131</v>
       </c>
-      <c r="B56" s="26" t="s">
+      <c r="B56" s="23" t="s">
         <v>190</v>
       </c>
       <c r="C56" s="16" t="s">
@@ -3608,7 +3622,7 @@
       <c r="E56" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F56" s="26" t="s">
+      <c r="F56" s="23" t="s">
         <v>368</v>
       </c>
     </row>
@@ -3616,7 +3630,7 @@
       <c r="A57" s="16">
         <v>129</v>
       </c>
-      <c r="B57" s="26" t="s">
+      <c r="B57" s="23" t="s">
         <v>188</v>
       </c>
       <c r="C57" s="16" t="s">
@@ -3628,7 +3642,7 @@
       <c r="E57" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F57" s="26" t="s">
+      <c r="F57" s="23" t="s">
         <v>440</v>
       </c>
     </row>
@@ -3636,7 +3650,7 @@
       <c r="A58" s="16">
         <v>130</v>
       </c>
-      <c r="B58" s="26" t="s">
+      <c r="B58" s="23" t="s">
         <v>189</v>
       </c>
       <c r="C58" s="16" t="s">
@@ -3648,7 +3662,7 @@
       <c r="E58" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F58" s="26" t="s">
+      <c r="F58" s="23" t="s">
         <v>367</v>
       </c>
     </row>
@@ -3656,7 +3670,7 @@
       <c r="A59" s="16">
         <v>122</v>
       </c>
-      <c r="B59" s="26" t="s">
+      <c r="B59" s="23" t="s">
         <v>181</v>
       </c>
       <c r="C59" s="16" t="s">
@@ -3668,19 +3682,19 @@
       <c r="E59" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="F59" s="26" t="s">
+      <c r="F59" s="23" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="17">
-        <v>134</v>
-      </c>
-      <c r="B60" s="27" t="s">
-        <v>194</v>
+        <v>137</v>
+      </c>
+      <c r="B60" s="24" t="s">
+        <v>197</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D60" s="17">
         <v>4</v>
@@ -3688,16 +3702,16 @@
       <c r="E60" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F60" s="27" t="s">
-        <v>370</v>
+      <c r="F60" s="24" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="17">
-        <v>133</v>
-      </c>
-      <c r="B61" s="27" t="s">
-        <v>193</v>
+        <v>135</v>
+      </c>
+      <c r="B61" s="24" t="s">
+        <v>195</v>
       </c>
       <c r="C61" s="17" t="s">
         <v>170</v>
@@ -3708,19 +3722,19 @@
       <c r="E61" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F61" s="27" t="s">
-        <v>441</v>
+      <c r="F61" s="24" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="17">
-        <v>132</v>
-      </c>
-      <c r="B62" s="27" t="s">
-        <v>191</v>
+        <v>136</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>196</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="D62" s="17">
         <v>4</v>
@@ -3728,19 +3742,19 @@
       <c r="E62" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F62" s="27" t="s">
-        <v>369</v>
+      <c r="F62" s="24" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="17">
-        <v>137</v>
-      </c>
-      <c r="B63" s="27" t="s">
-        <v>197</v>
+        <v>134</v>
+      </c>
+      <c r="B63" s="24" t="s">
+        <v>194</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D63" s="17">
         <v>4</v>
@@ -3748,16 +3762,16 @@
       <c r="E63" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F63" s="27" t="s">
-        <v>372</v>
+      <c r="F63" s="24" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="17">
-        <v>135</v>
-      </c>
-      <c r="B64" s="27" t="s">
-        <v>195</v>
+        <v>133</v>
+      </c>
+      <c r="B64" s="24" t="s">
+        <v>193</v>
       </c>
       <c r="C64" s="17" t="s">
         <v>170</v>
@@ -3768,19 +3782,19 @@
       <c r="E64" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F64" s="27" t="s">
-        <v>442</v>
+      <c r="F64" s="24" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="17">
-        <v>136</v>
-      </c>
-      <c r="B65" s="27" t="s">
-        <v>196</v>
+        <v>132</v>
+      </c>
+      <c r="B65" s="24" t="s">
+        <v>191</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="D65" s="17">
         <v>4</v>
@@ -3788,15 +3802,15 @@
       <c r="E65" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F65" s="27" t="s">
-        <v>371</v>
+      <c r="F65" s="24" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="17">
         <v>140</v>
       </c>
-      <c r="B66" s="27" t="s">
+      <c r="B66" s="24" t="s">
         <v>202</v>
       </c>
       <c r="C66" s="17" t="s">
@@ -3808,7 +3822,7 @@
       <c r="E66" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F66" s="27" t="s">
+      <c r="F66" s="24" t="s">
         <v>374</v>
       </c>
     </row>
@@ -3816,7 +3830,7 @@
       <c r="A67" s="17">
         <v>138</v>
       </c>
-      <c r="B67" s="27" t="s">
+      <c r="B67" s="24" t="s">
         <v>198</v>
       </c>
       <c r="C67" s="17" t="s">
@@ -3828,7 +3842,7 @@
       <c r="E67" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F67" s="27" t="s">
+      <c r="F67" s="24" t="s">
         <v>443</v>
       </c>
     </row>
@@ -3836,7 +3850,7 @@
       <c r="A68" s="17">
         <v>139</v>
       </c>
-      <c r="B68" s="27" t="s">
+      <c r="B68" s="24" t="s">
         <v>200</v>
       </c>
       <c r="C68" s="17" t="s">
@@ -3848,19 +3862,19 @@
       <c r="E68" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F68" s="27" t="s">
+      <c r="F68" s="24" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="17">
-        <v>144</v>
-      </c>
-      <c r="B69" s="27" t="s">
-        <v>207</v>
+        <v>147</v>
+      </c>
+      <c r="B69" s="24" t="s">
+        <v>210</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D69" s="17">
         <v>4</v>
@@ -3868,16 +3882,16 @@
       <c r="E69" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F69" s="27" t="s">
-        <v>377</v>
+      <c r="F69" s="24" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="17">
-        <v>143</v>
-      </c>
-      <c r="B70" s="27" t="s">
-        <v>206</v>
+        <v>145</v>
+      </c>
+      <c r="B70" s="24" t="s">
+        <v>208</v>
       </c>
       <c r="C70" s="17" t="s">
         <v>52</v>
@@ -3888,16 +3902,16 @@
       <c r="E70" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F70" s="27" t="s">
-        <v>444</v>
+      <c r="F70" s="24" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="17">
-        <v>142</v>
-      </c>
-      <c r="B71" s="27" t="s">
-        <v>205</v>
+        <v>146</v>
+      </c>
+      <c r="B71" s="24" t="s">
+        <v>209</v>
       </c>
       <c r="C71" s="17" t="s">
         <v>50</v>
@@ -3908,19 +3922,19 @@
       <c r="E71" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F71" s="27" t="s">
-        <v>376</v>
+      <c r="F71" s="24" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="17">
-        <v>147</v>
-      </c>
-      <c r="B72" s="27" t="s">
-        <v>210</v>
+        <v>144</v>
+      </c>
+      <c r="B72" s="24" t="s">
+        <v>207</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D72" s="17">
         <v>4</v>
@@ -3928,16 +3942,16 @@
       <c r="E72" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F72" s="27" t="s">
-        <v>379</v>
+      <c r="F72" s="24" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="17">
-        <v>145</v>
-      </c>
-      <c r="B73" s="27" t="s">
-        <v>208</v>
+        <v>143</v>
+      </c>
+      <c r="B73" s="24" t="s">
+        <v>206</v>
       </c>
       <c r="C73" s="17" t="s">
         <v>52</v>
@@ -3948,16 +3962,16 @@
       <c r="E73" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F73" s="27" t="s">
-        <v>445</v>
+      <c r="F73" s="24" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="17">
-        <v>146</v>
-      </c>
-      <c r="B74" s="27" t="s">
-        <v>209</v>
+        <v>142</v>
+      </c>
+      <c r="B74" s="24" t="s">
+        <v>205</v>
       </c>
       <c r="C74" s="17" t="s">
         <v>50</v>
@@ -3968,15 +3982,15 @@
       <c r="E74" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F74" s="27" t="s">
-        <v>378</v>
+      <c r="F74" s="24" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="17">
         <v>150</v>
       </c>
-      <c r="B75" s="27" t="s">
+      <c r="B75" s="24" t="s">
         <v>213</v>
       </c>
       <c r="C75" s="17" t="s">
@@ -3988,7 +4002,7 @@
       <c r="E75" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F75" s="27" t="s">
+      <c r="F75" s="24" t="s">
         <v>381</v>
       </c>
     </row>
@@ -3996,7 +4010,7 @@
       <c r="A76" s="17">
         <v>148</v>
       </c>
-      <c r="B76" s="27" t="s">
+      <c r="B76" s="24" t="s">
         <v>211</v>
       </c>
       <c r="C76" s="17" t="s">
@@ -4008,7 +4022,7 @@
       <c r="E76" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F76" s="27" t="s">
+      <c r="F76" s="24" t="s">
         <v>446</v>
       </c>
     </row>
@@ -4016,7 +4030,7 @@
       <c r="A77" s="17">
         <v>149</v>
       </c>
-      <c r="B77" s="27" t="s">
+      <c r="B77" s="24" t="s">
         <v>212</v>
       </c>
       <c r="C77" s="17" t="s">
@@ -4028,7 +4042,7 @@
       <c r="E77" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F77" s="27" t="s">
+      <c r="F77" s="24" t="s">
         <v>380</v>
       </c>
     </row>
@@ -4036,7 +4050,7 @@
       <c r="A78" s="17">
         <v>141</v>
       </c>
-      <c r="B78" s="27" t="s">
+      <c r="B78" s="24" t="s">
         <v>204</v>
       </c>
       <c r="C78" s="17" t="s">
@@ -4048,19 +4062,19 @@
       <c r="E78" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F78" s="27" t="s">
+      <c r="F78" s="24" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="17">
-        <v>154</v>
-      </c>
-      <c r="B79" s="27" t="s">
-        <v>218</v>
+        <v>157</v>
+      </c>
+      <c r="B79" s="24" t="s">
+        <v>221</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D79" s="17">
         <v>4</v>
@@ -4068,16 +4082,16 @@
       <c r="E79" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F79" s="27" t="s">
-        <v>384</v>
+      <c r="F79" s="24" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="17">
-        <v>153</v>
-      </c>
-      <c r="B80" s="27" t="s">
-        <v>217</v>
+        <v>155</v>
+      </c>
+      <c r="B80" s="24" t="s">
+        <v>219</v>
       </c>
       <c r="C80" s="17" t="s">
         <v>52</v>
@@ -4088,16 +4102,16 @@
       <c r="E80" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F80" s="27" t="s">
-        <v>447</v>
+      <c r="F80" s="24" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="17">
-        <v>152</v>
-      </c>
-      <c r="B81" s="27" t="s">
-        <v>216</v>
+        <v>156</v>
+      </c>
+      <c r="B81" s="24" t="s">
+        <v>220</v>
       </c>
       <c r="C81" s="17" t="s">
         <v>50</v>
@@ -4108,19 +4122,19 @@
       <c r="E81" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F81" s="27" t="s">
-        <v>383</v>
+      <c r="F81" s="24" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="17">
-        <v>157</v>
-      </c>
-      <c r="B82" s="27" t="s">
-        <v>221</v>
+        <v>154</v>
+      </c>
+      <c r="B82" s="24" t="s">
+        <v>218</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D82" s="17">
         <v>4</v>
@@ -4128,16 +4142,16 @@
       <c r="E82" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F82" s="27" t="s">
-        <v>386</v>
+      <c r="F82" s="24" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="17">
-        <v>155</v>
-      </c>
-      <c r="B83" s="27" t="s">
-        <v>219</v>
+        <v>153</v>
+      </c>
+      <c r="B83" s="24" t="s">
+        <v>217</v>
       </c>
       <c r="C83" s="17" t="s">
         <v>52</v>
@@ -4148,16 +4162,16 @@
       <c r="E83" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F83" s="27" t="s">
-        <v>448</v>
+      <c r="F83" s="24" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="17">
-        <v>156</v>
-      </c>
-      <c r="B84" s="27" t="s">
-        <v>220</v>
+        <v>152</v>
+      </c>
+      <c r="B84" s="24" t="s">
+        <v>216</v>
       </c>
       <c r="C84" s="17" t="s">
         <v>50</v>
@@ -4168,15 +4182,15 @@
       <c r="E84" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F84" s="27" t="s">
-        <v>385</v>
+      <c r="F84" s="24" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="17">
         <v>160</v>
       </c>
-      <c r="B85" s="27" t="s">
+      <c r="B85" s="24" t="s">
         <v>224</v>
       </c>
       <c r="C85" s="17" t="s">
@@ -4188,7 +4202,7 @@
       <c r="E85" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F85" s="27" t="s">
+      <c r="F85" s="24" t="s">
         <v>388</v>
       </c>
     </row>
@@ -4196,7 +4210,7 @@
       <c r="A86" s="17">
         <v>158</v>
       </c>
-      <c r="B86" s="27" t="s">
+      <c r="B86" s="24" t="s">
         <v>222</v>
       </c>
       <c r="C86" s="17" t="s">
@@ -4208,7 +4222,7 @@
       <c r="E86" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F86" s="27" t="s">
+      <c r="F86" s="24" t="s">
         <v>449</v>
       </c>
     </row>
@@ -4216,7 +4230,7 @@
       <c r="A87" s="17">
         <v>159</v>
       </c>
-      <c r="B87" s="27" t="s">
+      <c r="B87" s="24" t="s">
         <v>223</v>
       </c>
       <c r="C87" s="17" t="s">
@@ -4228,7 +4242,7 @@
       <c r="E87" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F87" s="27" t="s">
+      <c r="F87" s="24" t="s">
         <v>387</v>
       </c>
     </row>
@@ -4236,7 +4250,7 @@
       <c r="A88" s="17">
         <v>151</v>
       </c>
-      <c r="B88" s="27" t="s">
+      <c r="B88" s="24" t="s">
         <v>215</v>
       </c>
       <c r="C88" s="17" t="s">
@@ -4248,19 +4262,19 @@
       <c r="E88" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F88" s="27" t="s">
+      <c r="F88" s="24" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="17">
-        <v>164</v>
-      </c>
-      <c r="B89" s="27" t="s">
-        <v>228</v>
+        <v>167</v>
+      </c>
+      <c r="B89" s="24" t="s">
+        <v>231</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D89" s="17">
         <v>4</v>
@@ -4268,16 +4282,16 @@
       <c r="E89" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F89" s="27" t="s">
-        <v>391</v>
+      <c r="F89" s="24" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="17">
-        <v>163</v>
-      </c>
-      <c r="B90" s="27" t="s">
-        <v>227</v>
+        <v>165</v>
+      </c>
+      <c r="B90" s="24" t="s">
+        <v>229</v>
       </c>
       <c r="C90" s="17" t="s">
         <v>52</v>
@@ -4288,16 +4302,16 @@
       <c r="E90" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F90" s="27" t="s">
-        <v>450</v>
+      <c r="F90" s="24" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="17">
-        <v>162</v>
-      </c>
-      <c r="B91" s="27" t="s">
-        <v>226</v>
+        <v>166</v>
+      </c>
+      <c r="B91" s="24" t="s">
+        <v>230</v>
       </c>
       <c r="C91" s="17" t="s">
         <v>50</v>
@@ -4308,19 +4322,19 @@
       <c r="E91" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F91" s="27" t="s">
-        <v>390</v>
+      <c r="F91" s="24" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="17">
-        <v>167</v>
-      </c>
-      <c r="B92" s="27" t="s">
-        <v>231</v>
+        <v>164</v>
+      </c>
+      <c r="B92" s="24" t="s">
+        <v>228</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D92" s="17">
         <v>4</v>
@@ -4328,16 +4342,16 @@
       <c r="E92" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F92" s="27" t="s">
-        <v>393</v>
+      <c r="F92" s="24" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="17">
-        <v>165</v>
-      </c>
-      <c r="B93" s="27" t="s">
-        <v>229</v>
+        <v>163</v>
+      </c>
+      <c r="B93" s="24" t="s">
+        <v>227</v>
       </c>
       <c r="C93" s="17" t="s">
         <v>52</v>
@@ -4348,16 +4362,16 @@
       <c r="E93" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F93" s="27" t="s">
-        <v>451</v>
+      <c r="F93" s="24" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="17">
-        <v>166</v>
-      </c>
-      <c r="B94" s="27" t="s">
-        <v>230</v>
+        <v>162</v>
+      </c>
+      <c r="B94" s="24" t="s">
+        <v>226</v>
       </c>
       <c r="C94" s="17" t="s">
         <v>50</v>
@@ -4368,15 +4382,15 @@
       <c r="E94" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F94" s="27" t="s">
-        <v>392</v>
+      <c r="F94" s="24" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="17">
         <v>170</v>
       </c>
-      <c r="B95" s="27" t="s">
+      <c r="B95" s="24" t="s">
         <v>234</v>
       </c>
       <c r="C95" s="17" t="s">
@@ -4388,7 +4402,7 @@
       <c r="E95" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F95" s="27" t="s">
+      <c r="F95" s="24" t="s">
         <v>395</v>
       </c>
     </row>
@@ -4396,7 +4410,7 @@
       <c r="A96" s="17">
         <v>168</v>
       </c>
-      <c r="B96" s="27" t="s">
+      <c r="B96" s="24" t="s">
         <v>232</v>
       </c>
       <c r="C96" s="17" t="s">
@@ -4408,7 +4422,7 @@
       <c r="E96" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F96" s="27" t="s">
+      <c r="F96" s="24" t="s">
         <v>452</v>
       </c>
     </row>
@@ -4416,7 +4430,7 @@
       <c r="A97" s="17">
         <v>169</v>
       </c>
-      <c r="B97" s="27" t="s">
+      <c r="B97" s="24" t="s">
         <v>233</v>
       </c>
       <c r="C97" s="17" t="s">
@@ -4428,7 +4442,7 @@
       <c r="E97" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F97" s="27" t="s">
+      <c r="F97" s="24" t="s">
         <v>394</v>
       </c>
     </row>
@@ -4436,7 +4450,7 @@
       <c r="A98" s="17">
         <v>161</v>
       </c>
-      <c r="B98" s="27" t="s">
+      <c r="B98" s="24" t="s">
         <v>225</v>
       </c>
       <c r="C98" s="17" t="s">
@@ -4448,19 +4462,19 @@
       <c r="E98" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="F98" s="27" t="s">
+      <c r="F98" s="24" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="13">
-        <v>28</v>
-      </c>
-      <c r="B99" s="28" t="s">
-        <v>53</v>
+        <v>31</v>
+      </c>
+      <c r="B99" s="25" t="s">
+        <v>57</v>
       </c>
       <c r="C99" s="13" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D99" s="13">
         <v>5</v>
@@ -4468,16 +4482,16 @@
       <c r="E99" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F99" s="28" t="s">
-        <v>297</v>
+      <c r="F99" s="25" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="13">
-        <v>27</v>
-      </c>
-      <c r="B100" s="28" t="s">
-        <v>51</v>
+        <v>29</v>
+      </c>
+      <c r="B100" s="25" t="s">
+        <v>55</v>
       </c>
       <c r="C100" s="13" t="s">
         <v>52</v>
@@ -4488,16 +4502,16 @@
       <c r="E100" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F100" s="28" t="s">
-        <v>408</v>
+      <c r="F100" s="25" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="13">
-        <v>26</v>
-      </c>
-      <c r="B101" s="28" t="s">
-        <v>49</v>
+        <v>30</v>
+      </c>
+      <c r="B101" s="25" t="s">
+        <v>56</v>
       </c>
       <c r="C101" s="13" t="s">
         <v>50</v>
@@ -4508,19 +4522,19 @@
       <c r="E101" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F101" s="28" t="s">
-        <v>296</v>
+      <c r="F101" s="25" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="13">
-        <v>31</v>
-      </c>
-      <c r="B102" s="28" t="s">
-        <v>57</v>
+        <v>28</v>
+      </c>
+      <c r="B102" s="25" t="s">
+        <v>53</v>
       </c>
       <c r="C102" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D102" s="13">
         <v>5</v>
@@ -4528,16 +4542,16 @@
       <c r="E102" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F102" s="28" t="s">
-        <v>299</v>
+      <c r="F102" s="25" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="13">
-        <v>29</v>
-      </c>
-      <c r="B103" s="28" t="s">
-        <v>55</v>
+        <v>27</v>
+      </c>
+      <c r="B103" s="25" t="s">
+        <v>51</v>
       </c>
       <c r="C103" s="13" t="s">
         <v>52</v>
@@ -4548,16 +4562,16 @@
       <c r="E103" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F103" s="28" t="s">
-        <v>409</v>
+      <c r="F103" s="25" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="13">
-        <v>30</v>
-      </c>
-      <c r="B104" s="28" t="s">
-        <v>56</v>
+        <v>26</v>
+      </c>
+      <c r="B104" s="25" t="s">
+        <v>49</v>
       </c>
       <c r="C104" s="13" t="s">
         <v>50</v>
@@ -4568,15 +4582,15 @@
       <c r="E104" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F104" s="28" t="s">
-        <v>298</v>
+      <c r="F104" s="25" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="13">
         <v>34</v>
       </c>
-      <c r="B105" s="28" t="s">
+      <c r="B105" s="25" t="s">
         <v>62</v>
       </c>
       <c r="C105" s="13" t="s">
@@ -4588,7 +4602,7 @@
       <c r="E105" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F105" s="28" t="s">
+      <c r="F105" s="25" t="s">
         <v>301</v>
       </c>
     </row>
@@ -4596,7 +4610,7 @@
       <c r="A106" s="13">
         <v>32</v>
       </c>
-      <c r="B106" s="28" t="s">
+      <c r="B106" s="25" t="s">
         <v>59</v>
       </c>
       <c r="C106" s="13" t="s">
@@ -4608,7 +4622,7 @@
       <c r="E106" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F106" s="28" t="s">
+      <c r="F106" s="25" t="s">
         <v>410</v>
       </c>
     </row>
@@ -4616,7 +4630,7 @@
       <c r="A107" s="13">
         <v>33</v>
       </c>
-      <c r="B107" s="28" t="s">
+      <c r="B107" s="25" t="s">
         <v>60</v>
       </c>
       <c r="C107" s="13" t="s">
@@ -4628,19 +4642,19 @@
       <c r="E107" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F107" s="28" t="s">
+      <c r="F107" s="25" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="13">
-        <v>38</v>
-      </c>
-      <c r="B108" s="28" t="s">
-        <v>69</v>
+        <v>41</v>
+      </c>
+      <c r="B108" s="25" t="s">
+        <v>73</v>
       </c>
       <c r="C108" s="13" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D108" s="13">
         <v>5</v>
@@ -4648,16 +4662,16 @@
       <c r="E108" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F108" s="28" t="s">
-        <v>304</v>
+      <c r="F108" s="25" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="13">
-        <v>37</v>
-      </c>
-      <c r="B109" s="28" t="s">
-        <v>67</v>
+        <v>39</v>
+      </c>
+      <c r="B109" s="25" t="s">
+        <v>71</v>
       </c>
       <c r="C109" s="13" t="s">
         <v>68</v>
@@ -4668,16 +4682,16 @@
       <c r="E109" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F109" s="28" t="s">
-        <v>411</v>
+      <c r="F109" s="25" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="13">
-        <v>36</v>
-      </c>
-      <c r="B110" s="28" t="s">
-        <v>65</v>
+        <v>40</v>
+      </c>
+      <c r="B110" s="25" t="s">
+        <v>72</v>
       </c>
       <c r="C110" s="13" t="s">
         <v>66</v>
@@ -4688,19 +4702,19 @@
       <c r="E110" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F110" s="28" t="s">
-        <v>303</v>
+      <c r="F110" s="25" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="13">
-        <v>41</v>
-      </c>
-      <c r="B111" s="28" t="s">
-        <v>73</v>
+        <v>38</v>
+      </c>
+      <c r="B111" s="25" t="s">
+        <v>69</v>
       </c>
       <c r="C111" s="13" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D111" s="13">
         <v>5</v>
@@ -4708,16 +4722,16 @@
       <c r="E111" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F111" s="28" t="s">
-        <v>306</v>
+      <c r="F111" s="25" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="13">
-        <v>39</v>
-      </c>
-      <c r="B112" s="28" t="s">
-        <v>71</v>
+        <v>37</v>
+      </c>
+      <c r="B112" s="25" t="s">
+        <v>67</v>
       </c>
       <c r="C112" s="13" t="s">
         <v>68</v>
@@ -4728,16 +4742,16 @@
       <c r="E112" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F112" s="28" t="s">
-        <v>412</v>
+      <c r="F112" s="25" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="13">
-        <v>40</v>
-      </c>
-      <c r="B113" s="28" t="s">
-        <v>72</v>
+        <v>36</v>
+      </c>
+      <c r="B113" s="25" t="s">
+        <v>65</v>
       </c>
       <c r="C113" s="13" t="s">
         <v>66</v>
@@ -4748,15 +4762,15 @@
       <c r="E113" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F113" s="28" t="s">
-        <v>305</v>
+      <c r="F113" s="25" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="13">
         <v>44</v>
       </c>
-      <c r="B114" s="28" t="s">
+      <c r="B114" s="25" t="s">
         <v>77</v>
       </c>
       <c r="C114" s="13" t="s">
@@ -4768,7 +4782,7 @@
       <c r="E114" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F114" s="28" t="s">
+      <c r="F114" s="25" t="s">
         <v>308</v>
       </c>
     </row>
@@ -4776,7 +4790,7 @@
       <c r="A115" s="13">
         <v>42</v>
       </c>
-      <c r="B115" s="28" t="s">
+      <c r="B115" s="25" t="s">
         <v>75</v>
       </c>
       <c r="C115" s="13" t="s">
@@ -4788,7 +4802,7 @@
       <c r="E115" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F115" s="28" t="s">
+      <c r="F115" s="25" t="s">
         <v>413</v>
       </c>
     </row>
@@ -4796,7 +4810,7 @@
       <c r="A116" s="13">
         <v>43</v>
       </c>
-      <c r="B116" s="28" t="s">
+      <c r="B116" s="25" t="s">
         <v>76</v>
       </c>
       <c r="C116" s="13" t="s">
@@ -4808,7 +4822,7 @@
       <c r="E116" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F116" s="28" t="s">
+      <c r="F116" s="25" t="s">
         <v>307</v>
       </c>
     </row>
@@ -4816,7 +4830,7 @@
       <c r="A117" s="13">
         <v>35</v>
       </c>
-      <c r="B117" s="28" t="s">
+      <c r="B117" s="25" t="s">
         <v>64</v>
       </c>
       <c r="C117" s="13" t="s">
@@ -4828,19 +4842,19 @@
       <c r="E117" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F117" s="28" t="s">
+      <c r="F117" s="25" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="13">
-        <v>45</v>
-      </c>
-      <c r="B118" s="28" t="s">
-        <v>79</v>
+        <v>51</v>
+      </c>
+      <c r="B118" s="25" t="s">
+        <v>85</v>
       </c>
       <c r="C118" s="13" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="D118" s="13">
         <v>5</v>
@@ -4848,19 +4862,19 @@
       <c r="E118" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F118" s="28" t="s">
-        <v>309</v>
+      <c r="F118" s="25" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="13">
-        <v>48</v>
-      </c>
-      <c r="B119" s="28" t="s">
-        <v>82</v>
+        <v>49</v>
+      </c>
+      <c r="B119" s="25" t="s">
+        <v>83</v>
       </c>
       <c r="C119" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D119" s="13">
         <v>5</v>
@@ -4868,19 +4882,19 @@
       <c r="E119" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F119" s="28" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F119" s="25" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="13">
-        <v>47</v>
-      </c>
-      <c r="B120" s="28" t="s">
-        <v>81</v>
+        <v>50</v>
+      </c>
+      <c r="B120" s="25" t="s">
+        <v>84</v>
       </c>
       <c r="C120" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D120" s="13">
         <v>5</v>
@@ -4888,19 +4902,19 @@
       <c r="E120" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F120" s="28" t="s">
-        <v>414</v>
+      <c r="F120" s="25" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="13">
-        <v>46</v>
-      </c>
-      <c r="B121" s="28" t="s">
-        <v>80</v>
+        <v>48</v>
+      </c>
+      <c r="B121" s="25" t="s">
+        <v>82</v>
       </c>
       <c r="C121" s="13" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D121" s="13">
         <v>5</v>
@@ -4908,19 +4922,19 @@
       <c r="E121" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F121" s="28" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F121" s="25" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="13">
-        <v>51</v>
-      </c>
-      <c r="B122" s="28" t="s">
-        <v>85</v>
+        <v>47</v>
+      </c>
+      <c r="B122" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="C122" s="13" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D122" s="13">
         <v>5</v>
@@ -4928,19 +4942,19 @@
       <c r="E122" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F122" s="28" t="s">
-        <v>313</v>
+      <c r="F122" s="25" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="13">
-        <v>49</v>
-      </c>
-      <c r="B123" s="28" t="s">
-        <v>83</v>
+        <v>46</v>
+      </c>
+      <c r="B123" s="25" t="s">
+        <v>80</v>
       </c>
       <c r="C123" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D123" s="13">
         <v>5</v>
@@ -4948,19 +4962,19 @@
       <c r="E123" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F123" s="28" t="s">
-        <v>415</v>
+      <c r="F123" s="25" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="13">
-        <v>50</v>
-      </c>
-      <c r="B124" s="28" t="s">
-        <v>84</v>
+        <v>54</v>
+      </c>
+      <c r="B124" s="25" t="s">
+        <v>88</v>
       </c>
       <c r="C124" s="13" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="D124" s="13">
         <v>5</v>
@@ -4968,19 +4982,19 @@
       <c r="E124" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F124" s="28" t="s">
-        <v>312</v>
+      <c r="F124" s="25" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="13">
-        <v>54</v>
-      </c>
-      <c r="B125" s="28" t="s">
-        <v>88</v>
+        <v>52</v>
+      </c>
+      <c r="B125" s="25" t="s">
+        <v>86</v>
       </c>
       <c r="C125" s="13" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="D125" s="13">
         <v>5</v>
@@ -4988,19 +5002,19 @@
       <c r="E125" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F125" s="28" t="s">
-        <v>315</v>
+      <c r="F125" s="25" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="13">
-        <v>52</v>
-      </c>
-      <c r="B126" s="28" t="s">
-        <v>86</v>
+        <v>53</v>
+      </c>
+      <c r="B126" s="25" t="s">
+        <v>87</v>
       </c>
       <c r="C126" s="13" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D126" s="13">
         <v>5</v>
@@ -5008,16 +5022,16 @@
       <c r="E126" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F126" s="28" t="s">
-        <v>416</v>
+      <c r="F126" s="25" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="13">
-        <v>53</v>
-      </c>
-      <c r="B127" s="28" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="B127" s="25" t="s">
+        <v>79</v>
       </c>
       <c r="C127" s="13" t="s">
         <v>61</v>
@@ -5028,19 +5042,19 @@
       <c r="E127" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F127" s="28" t="s">
-        <v>314</v>
+      <c r="F127" s="25" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="14">
-        <v>57</v>
-      </c>
-      <c r="B128" s="29" t="s">
-        <v>92</v>
+        <v>60</v>
+      </c>
+      <c r="B128" s="26" t="s">
+        <v>95</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D128" s="14">
         <v>6</v>
@@ -5048,16 +5062,16 @@
       <c r="E128" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F128" s="29" t="s">
-        <v>317</v>
+      <c r="F128" s="26" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="14">
-        <v>56</v>
-      </c>
-      <c r="B129" s="29" t="s">
-        <v>91</v>
+        <v>58</v>
+      </c>
+      <c r="B129" s="26" t="s">
+        <v>93</v>
       </c>
       <c r="C129" s="14" t="s">
         <v>68</v>
@@ -5068,19 +5082,19 @@
       <c r="E129" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F129" s="29" t="s">
-        <v>417</v>
+      <c r="F129" s="26" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="14">
-        <v>55</v>
-      </c>
-      <c r="B130" s="29" t="s">
-        <v>89</v>
+        <v>59</v>
+      </c>
+      <c r="B130" s="26" t="s">
+        <v>94</v>
       </c>
       <c r="C130" s="14" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="D130" s="14">
         <v>6</v>
@@ -5088,19 +5102,19 @@
       <c r="E130" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F130" s="29" t="s">
-        <v>316</v>
+      <c r="F130" s="26" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="14">
-        <v>60</v>
-      </c>
-      <c r="B131" s="29" t="s">
-        <v>95</v>
+        <v>57</v>
+      </c>
+      <c r="B131" s="26" t="s">
+        <v>92</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D131" s="14">
         <v>6</v>
@@ -5108,16 +5122,16 @@
       <c r="E131" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F131" s="29" t="s">
-        <v>319</v>
+      <c r="F131" s="26" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="14">
-        <v>58</v>
-      </c>
-      <c r="B132" s="29" t="s">
-        <v>93</v>
+        <v>56</v>
+      </c>
+      <c r="B132" s="26" t="s">
+        <v>91</v>
       </c>
       <c r="C132" s="14" t="s">
         <v>68</v>
@@ -5128,19 +5142,19 @@
       <c r="E132" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F132" s="29" t="s">
-        <v>418</v>
+      <c r="F132" s="26" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="14">
-        <v>59</v>
-      </c>
-      <c r="B133" s="29" t="s">
-        <v>94</v>
+        <v>55</v>
+      </c>
+      <c r="B133" s="26" t="s">
+        <v>89</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="D133" s="14">
         <v>6</v>
@@ -5148,15 +5162,15 @@
       <c r="E133" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F133" s="29" t="s">
-        <v>318</v>
+      <c r="F133" s="26" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="14">
         <v>63</v>
       </c>
-      <c r="B134" s="29" t="s">
+      <c r="B134" s="26" t="s">
         <v>100</v>
       </c>
       <c r="C134" s="14" t="s">
@@ -5168,7 +5182,7 @@
       <c r="E134" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F134" s="29" t="s">
+      <c r="F134" s="26" t="s">
         <v>321</v>
       </c>
     </row>
@@ -5176,7 +5190,7 @@
       <c r="A135" s="14">
         <v>61</v>
       </c>
-      <c r="B135" s="29" t="s">
+      <c r="B135" s="26" t="s">
         <v>96</v>
       </c>
       <c r="C135" s="14" t="s">
@@ -5188,7 +5202,7 @@
       <c r="E135" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F135" s="29" t="s">
+      <c r="F135" s="26" t="s">
         <v>419</v>
       </c>
     </row>
@@ -5196,7 +5210,7 @@
       <c r="A136" s="14">
         <v>62</v>
       </c>
-      <c r="B136" s="29" t="s">
+      <c r="B136" s="26" t="s">
         <v>98</v>
       </c>
       <c r="C136" s="14" t="s">
@@ -5208,19 +5222,19 @@
       <c r="E136" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F136" s="29" t="s">
+      <c r="F136" s="26" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" s="14">
-        <v>67</v>
-      </c>
-      <c r="B137" s="29" t="s">
-        <v>107</v>
+        <v>70</v>
+      </c>
+      <c r="B137" s="26" t="s">
+        <v>111</v>
       </c>
       <c r="C137" s="14" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D137" s="14">
         <v>6</v>
@@ -5228,16 +5242,16 @@
       <c r="E137" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F137" s="29" t="s">
-        <v>324</v>
+      <c r="F137" s="26" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="14">
-        <v>66</v>
-      </c>
-      <c r="B138" s="29" t="s">
-        <v>105</v>
+        <v>68</v>
+      </c>
+      <c r="B138" s="26" t="s">
+        <v>109</v>
       </c>
       <c r="C138" s="14" t="s">
         <v>106</v>
@@ -5248,16 +5262,16 @@
       <c r="E138" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F138" s="29" t="s">
-        <v>420</v>
+      <c r="F138" s="26" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="14">
-        <v>65</v>
-      </c>
-      <c r="B139" s="29" t="s">
-        <v>103</v>
+        <v>69</v>
+      </c>
+      <c r="B139" s="26" t="s">
+        <v>110</v>
       </c>
       <c r="C139" s="14" t="s">
         <v>104</v>
@@ -5268,19 +5282,19 @@
       <c r="E139" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F139" s="29" t="s">
-        <v>323</v>
+      <c r="F139" s="26" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="14">
-        <v>70</v>
-      </c>
-      <c r="B140" s="29" t="s">
-        <v>111</v>
+        <v>67</v>
+      </c>
+      <c r="B140" s="26" t="s">
+        <v>107</v>
       </c>
       <c r="C140" s="14" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D140" s="14">
         <v>6</v>
@@ -5288,16 +5302,16 @@
       <c r="E140" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F140" s="29" t="s">
-        <v>326</v>
+      <c r="F140" s="26" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="14">
-        <v>68</v>
-      </c>
-      <c r="B141" s="29" t="s">
-        <v>109</v>
+        <v>66</v>
+      </c>
+      <c r="B141" s="26" t="s">
+        <v>105</v>
       </c>
       <c r="C141" s="14" t="s">
         <v>106</v>
@@ -5308,16 +5322,16 @@
       <c r="E141" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F141" s="29" t="s">
-        <v>421</v>
+      <c r="F141" s="26" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="14">
-        <v>69</v>
-      </c>
-      <c r="B142" s="29" t="s">
-        <v>110</v>
+        <v>65</v>
+      </c>
+      <c r="B142" s="26" t="s">
+        <v>103</v>
       </c>
       <c r="C142" s="14" t="s">
         <v>104</v>
@@ -5328,15 +5342,15 @@
       <c r="E142" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F142" s="29" t="s">
-        <v>325</v>
+      <c r="F142" s="26" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="14">
         <v>73</v>
       </c>
-      <c r="B143" s="29" t="s">
+      <c r="B143" s="26" t="s">
         <v>115</v>
       </c>
       <c r="C143" s="14" t="s">
@@ -5348,7 +5362,7 @@
       <c r="E143" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F143" s="29" t="s">
+      <c r="F143" s="26" t="s">
         <v>328</v>
       </c>
     </row>
@@ -5356,7 +5370,7 @@
       <c r="A144" s="14">
         <v>71</v>
       </c>
-      <c r="B144" s="29" t="s">
+      <c r="B144" s="26" t="s">
         <v>113</v>
       </c>
       <c r="C144" s="14" t="s">
@@ -5368,7 +5382,7 @@
       <c r="E144" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F144" s="29" t="s">
+      <c r="F144" s="26" t="s">
         <v>422</v>
       </c>
     </row>
@@ -5376,7 +5390,7 @@
       <c r="A145" s="14">
         <v>72</v>
       </c>
-      <c r="B145" s="29" t="s">
+      <c r="B145" s="26" t="s">
         <v>114</v>
       </c>
       <c r="C145" s="14" t="s">
@@ -5388,7 +5402,7 @@
       <c r="E145" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F145" s="29" t="s">
+      <c r="F145" s="26" t="s">
         <v>327</v>
       </c>
     </row>
@@ -5396,7 +5410,7 @@
       <c r="A146" s="14">
         <v>64</v>
       </c>
-      <c r="B146" s="29" t="s">
+      <c r="B146" s="26" t="s">
         <v>102</v>
       </c>
       <c r="C146" s="14" t="s">
@@ -5408,19 +5422,19 @@
       <c r="E146" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F146" s="29" t="s">
+      <c r="F146" s="26" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="14">
-        <v>77</v>
-      </c>
-      <c r="B147" s="29" t="s">
-        <v>120</v>
+        <v>80</v>
+      </c>
+      <c r="B147" s="26" t="s">
+        <v>123</v>
       </c>
       <c r="C147" s="14" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D147" s="14">
         <v>6</v>
@@ -5428,16 +5442,16 @@
       <c r="E147" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F147" s="29" t="s">
-        <v>331</v>
+      <c r="F147" s="26" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="14">
-        <v>76</v>
-      </c>
-      <c r="B148" s="29" t="s">
-        <v>119</v>
+        <v>78</v>
+      </c>
+      <c r="B148" s="26" t="s">
+        <v>121</v>
       </c>
       <c r="C148" s="14" t="s">
         <v>106</v>
@@ -5448,16 +5462,16 @@
       <c r="E148" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F148" s="29" t="s">
-        <v>423</v>
+      <c r="F148" s="26" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="14">
-        <v>75</v>
-      </c>
-      <c r="B149" s="29" t="s">
-        <v>118</v>
+        <v>79</v>
+      </c>
+      <c r="B149" s="26" t="s">
+        <v>122</v>
       </c>
       <c r="C149" s="14" t="s">
         <v>104</v>
@@ -5468,19 +5482,19 @@
       <c r="E149" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F149" s="29" t="s">
-        <v>330</v>
+      <c r="F149" s="26" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="14">
-        <v>80</v>
-      </c>
-      <c r="B150" s="29" t="s">
-        <v>123</v>
+        <v>77</v>
+      </c>
+      <c r="B150" s="26" t="s">
+        <v>120</v>
       </c>
       <c r="C150" s="14" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D150" s="14">
         <v>6</v>
@@ -5488,16 +5502,16 @@
       <c r="E150" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F150" s="29" t="s">
-        <v>333</v>
+      <c r="F150" s="26" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="14">
-        <v>78</v>
-      </c>
-      <c r="B151" s="29" t="s">
-        <v>121</v>
+        <v>76</v>
+      </c>
+      <c r="B151" s="26" t="s">
+        <v>119</v>
       </c>
       <c r="C151" s="14" t="s">
         <v>106</v>
@@ -5508,16 +5522,16 @@
       <c r="E151" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F151" s="29" t="s">
-        <v>424</v>
+      <c r="F151" s="26" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="14">
-        <v>79</v>
-      </c>
-      <c r="B152" s="29" t="s">
-        <v>122</v>
+        <v>75</v>
+      </c>
+      <c r="B152" s="26" t="s">
+        <v>118</v>
       </c>
       <c r="C152" s="14" t="s">
         <v>104</v>
@@ -5528,15 +5542,15 @@
       <c r="E152" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F152" s="29" t="s">
-        <v>332</v>
+      <c r="F152" s="26" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="14">
         <v>83</v>
       </c>
-      <c r="B153" s="29" t="s">
+      <c r="B153" s="26" t="s">
         <v>126</v>
       </c>
       <c r="C153" s="14" t="s">
@@ -5548,7 +5562,7 @@
       <c r="E153" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F153" s="29" t="s">
+      <c r="F153" s="26" t="s">
         <v>335</v>
       </c>
     </row>
@@ -5556,7 +5570,7 @@
       <c r="A154" s="14">
         <v>81</v>
       </c>
-      <c r="B154" s="29" t="s">
+      <c r="B154" s="26" t="s">
         <v>124</v>
       </c>
       <c r="C154" s="14" t="s">
@@ -5568,7 +5582,7 @@
       <c r="E154" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F154" s="29" t="s">
+      <c r="F154" s="26" t="s">
         <v>425</v>
       </c>
     </row>
@@ -5576,7 +5590,7 @@
       <c r="A155" s="14">
         <v>82</v>
       </c>
-      <c r="B155" s="29" t="s">
+      <c r="B155" s="26" t="s">
         <v>125</v>
       </c>
       <c r="C155" s="14" t="s">
@@ -5588,7 +5602,7 @@
       <c r="E155" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F155" s="29" t="s">
+      <c r="F155" s="26" t="s">
         <v>334</v>
       </c>
     </row>
@@ -5596,7 +5610,7 @@
       <c r="A156" s="14">
         <v>74</v>
       </c>
-      <c r="B156" s="29" t="s">
+      <c r="B156" s="26" t="s">
         <v>117</v>
       </c>
       <c r="C156" s="14" t="s">
@@ -5608,79 +5622,79 @@
       <c r="E156" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="F156" s="29" t="s">
+      <c r="F156" s="26" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A157" s="15">
-        <v>86</v>
-      </c>
-      <c r="B157" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="C157" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D157" s="15">
+    <row r="157" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="36">
+        <v>89</v>
+      </c>
+      <c r="B157" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C157" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D157" s="36">
         <v>7</v>
       </c>
-      <c r="E157" s="15" t="s">
+      <c r="E157" s="36" t="s">
         <v>273</v>
       </c>
-      <c r="F157" s="30" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A158" s="15">
-        <v>85</v>
-      </c>
-      <c r="B158" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="C158" s="15" t="s">
+      <c r="F157" s="37" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="36">
+        <v>87</v>
+      </c>
+      <c r="B158" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C158" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="D158" s="15">
+      <c r="D158" s="36">
         <v>7</v>
       </c>
-      <c r="E158" s="15" t="s">
+      <c r="E158" s="36" t="s">
         <v>273</v>
       </c>
-      <c r="F158" s="30" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A159" s="15">
-        <v>84</v>
-      </c>
-      <c r="B159" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="C159" s="15" t="s">
+      <c r="F158" s="37" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="36">
+        <v>88</v>
+      </c>
+      <c r="B159" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="C159" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="D159" s="15">
+      <c r="D159" s="36">
         <v>7</v>
       </c>
-      <c r="E159" s="15" t="s">
+      <c r="E159" s="36" t="s">
         <v>273</v>
       </c>
-      <c r="F159" s="30" t="s">
-        <v>336</v>
+      <c r="F159" s="37" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="15">
-        <v>89</v>
-      </c>
-      <c r="B160" s="30" t="s">
-        <v>132</v>
+        <v>86</v>
+      </c>
+      <c r="B160" s="27" t="s">
+        <v>129</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D160" s="15">
         <v>7</v>
@@ -5688,16 +5702,16 @@
       <c r="E160" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="F160" s="30" t="s">
-        <v>339</v>
+      <c r="F160" s="27" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="15">
-        <v>87</v>
-      </c>
-      <c r="B161" s="30" t="s">
-        <v>130</v>
+        <v>85</v>
+      </c>
+      <c r="B161" s="27" t="s">
+        <v>128</v>
       </c>
       <c r="C161" s="15" t="s">
         <v>106</v>
@@ -5708,16 +5722,16 @@
       <c r="E161" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="F161" s="30" t="s">
-        <v>427</v>
+      <c r="F161" s="27" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="15">
-        <v>88</v>
-      </c>
-      <c r="B162" s="30" t="s">
-        <v>131</v>
+        <v>84</v>
+      </c>
+      <c r="B162" s="27" t="s">
+        <v>127</v>
       </c>
       <c r="C162" s="15" t="s">
         <v>104</v>
@@ -5728,15 +5742,15 @@
       <c r="E162" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="F162" s="30" t="s">
-        <v>338</v>
+      <c r="F162" s="27" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="15">
         <v>92</v>
       </c>
-      <c r="B163" s="30" t="s">
+      <c r="B163" s="27" t="s">
         <v>137</v>
       </c>
       <c r="C163" s="15" t="s">
@@ -5748,7 +5762,7 @@
       <c r="E163" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="F163" s="30" t="s">
+      <c r="F163" s="27" t="s">
         <v>341</v>
       </c>
     </row>
@@ -5756,7 +5770,7 @@
       <c r="A164" s="15">
         <v>90</v>
       </c>
-      <c r="B164" s="30" t="s">
+      <c r="B164" s="27" t="s">
         <v>133</v>
       </c>
       <c r="C164" s="15" t="s">
@@ -5768,7 +5782,7 @@
       <c r="E164" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="F164" s="30" t="s">
+      <c r="F164" s="27" t="s">
         <v>428</v>
       </c>
     </row>
@@ -5776,7 +5790,7 @@
       <c r="A165" s="15">
         <v>91</v>
       </c>
-      <c r="B165" s="30" t="s">
+      <c r="B165" s="27" t="s">
         <v>135</v>
       </c>
       <c r="C165" s="15" t="s">
@@ -5788,7 +5802,7 @@
       <c r="E165" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="F165" s="30" t="s">
+      <c r="F165" s="27" t="s">
         <v>340</v>
       </c>
     </row>
@@ -5796,7 +5810,7 @@
       <c r="A166" s="9">
         <v>5</v>
       </c>
-      <c r="B166" s="31" t="s">
+      <c r="B166" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C166" s="9" t="s">
@@ -5808,7 +5822,7 @@
       <c r="E166" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F166" s="31" t="s">
+      <c r="F166" s="28" t="s">
         <v>282</v>
       </c>
     </row>
@@ -5816,7 +5830,7 @@
       <c r="A167" s="9">
         <v>3</v>
       </c>
-      <c r="B167" s="31" t="s">
+      <c r="B167" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C167" s="9" t="s">
@@ -5828,7 +5842,7 @@
       <c r="E167" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F167" s="31" t="s">
+      <c r="F167" s="28" t="s">
         <v>400</v>
       </c>
     </row>
@@ -5836,7 +5850,7 @@
       <c r="A168" s="9">
         <v>4</v>
       </c>
-      <c r="B168" s="31" t="s">
+      <c r="B168" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C168" s="9" t="s">
@@ -5848,7 +5862,7 @@
       <c r="E168" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F168" s="31" t="s">
+      <c r="F168" s="28" t="s">
         <v>281</v>
       </c>
     </row>
@@ -5856,7 +5870,7 @@
       <c r="A169" s="10">
         <v>6</v>
       </c>
-      <c r="B169" s="32" t="s">
+      <c r="B169" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C169" s="10" t="s">
@@ -5868,7 +5882,7 @@
       <c r="E169" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="F169" s="32" t="s">
+      <c r="F169" s="29" t="s">
         <v>283</v>
       </c>
     </row>
@@ -5876,7 +5890,7 @@
       <c r="A170" s="11">
         <v>9</v>
       </c>
-      <c r="B170" s="33" t="s">
+      <c r="B170" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C170" s="11" t="s">
@@ -5888,7 +5902,7 @@
       <c r="E170" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="F170" s="33" t="s">
+      <c r="F170" s="30" t="s">
         <v>285</v>
       </c>
     </row>
@@ -5896,7 +5910,7 @@
       <c r="A171" s="11">
         <v>8</v>
       </c>
-      <c r="B171" s="33" t="s">
+      <c r="B171" s="30" t="s">
         <v>16</v>
       </c>
       <c r="C171" s="11" t="s">
@@ -5908,7 +5922,7 @@
       <c r="E171" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="F171" s="33" t="s">
+      <c r="F171" s="30" t="s">
         <v>401</v>
       </c>
     </row>
@@ -5916,7 +5930,7 @@
       <c r="A172" s="11">
         <v>7</v>
       </c>
-      <c r="B172" s="33" t="s">
+      <c r="B172" s="30" t="s">
         <v>14</v>
       </c>
       <c r="C172" s="11" t="s">
@@ -5928,7 +5942,7 @@
       <c r="E172" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="F172" s="33" t="s">
+      <c r="F172" s="30" t="s">
         <v>284</v>
       </c>
     </row>
@@ -5936,7 +5950,7 @@
       <c r="A173" s="11">
         <v>10</v>
       </c>
-      <c r="B173" s="33" t="s">
+      <c r="B173" s="30" t="s">
         <v>20</v>
       </c>
       <c r="C173" s="11" t="s">
@@ -5948,7 +5962,7 @@
       <c r="E173" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="F173" s="33" t="s">
+      <c r="F173" s="30" t="s">
         <v>402</v>
       </c>
     </row>
@@ -5956,7 +5970,7 @@
       <c r="A174" s="18">
         <v>172</v>
       </c>
-      <c r="B174" s="22" t="s">
+      <c r="B174" s="19" t="s">
         <v>237</v>
       </c>
       <c r="C174" s="18" t="s">
@@ -5968,7 +5982,7 @@
       <c r="E174" s="18" t="s">
         <v>277</v>
       </c>
-      <c r="F174" s="22" t="s">
+      <c r="F174" s="19" t="s">
         <v>397</v>
       </c>
     </row>
@@ -5981,8 +5995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView zoomScale="164" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5994,15 +6008,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="34" t="s">
         <v>262</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -6285,52 +6299,52 @@
       <c r="B14" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="33" t="s">
         <v>264</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="33" t="s">
         <v>265</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="33" t="s">
         <v>266</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>

</xml_diff>